<commit_message>
Update DR# 630 Veterans Bank(Ribbon)_01_11_2021.xlsx
</commit_message>
<xml_diff>
--- a/DR# 630 Veterans Bank(Ribbon)_01_11_2021.xlsx
+++ b/DR# 630 Veterans Bank(Ribbon)_01_11_2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAAAB32E-F04B-4C90-98B8-B3BFE4B319A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E56F7E-FB11-409B-9AE4-54723FDB0F83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1379,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1523,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="38">
-        <v>44501</v>
+        <v>44531</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18">

</xml_diff>